<commit_message>
A commit before report
</commit_message>
<xml_diff>
--- a/Report/Report/Network Width to Accuracy.xlsx
+++ b/Report/Report/Network Width to Accuracy.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -3649,16 +3649,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>